<commit_message>
Se adicionan los ejemplos creados por Jeison
</commit_message>
<xml_diff>
--- a/taller arq.xlsx
+++ b/taller arq.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas Salazar\Documents\Universidad\Semestre 7\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nelsonpinzon/Library/Mobile Documents/com~apple~CloudDocs/Documents/Especialización/Arquitectura de Software/Software-Architecture/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60B94E6E-9C04-4854-9DE6-2D278B58D17A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76E34344-8234-CD40-B3C6-82652A126FBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{930C2BC0-64CF-D141-82C4-9B5BCF2C150D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{930C2BC0-64CF-D141-82C4-9B5BCF2C150D}"/>
   </bookViews>
   <sheets>
     <sheet name="QA" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="62">
   <si>
     <t>Atributos Calidad</t>
   </si>
@@ -162,9 +162,6 @@
     <t>Software</t>
   </si>
   <si>
-    <t>Notificar al area de servidor}</t>
-  </si>
-  <si>
     <t>Componente defectuoso</t>
   </si>
   <si>
@@ -202,6 +199,27 @@
   </si>
   <si>
     <t>En ejecución</t>
+  </si>
+  <si>
+    <t>Ingreso del cliente para la cotización</t>
+  </si>
+  <si>
+    <t>Verificar la autenticidad del cliente</t>
+  </si>
+  <si>
+    <t>1 hora</t>
+  </si>
+  <si>
+    <t>Interoperability</t>
+  </si>
+  <si>
+    <t>Respuesta del servicio en linea</t>
+  </si>
+  <si>
+    <t>Verificar la respuesta a la cotización</t>
+  </si>
+  <si>
+    <t>Notificar al area de servidor</t>
   </si>
 </sst>
 </file>
@@ -304,7 +322,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -335,10 +353,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -350,10 +365,16 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -671,21 +692,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30A29C82-537D-0A41-8469-EA9B4533FFF4}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.875" customWidth="1"/>
-    <col min="2" max="2" width="53.875" customWidth="1"/>
-    <col min="3" max="3" width="38.125" customWidth="1"/>
-    <col min="4" max="4" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.83203125" customWidth="1"/>
+    <col min="2" max="2" width="53.83203125" customWidth="1"/>
+    <col min="3" max="3" width="38.1640625" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -696,14 +717,14 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
     </row>
-    <row r="3" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -714,7 +735,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -725,7 +746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -736,7 +757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -747,7 +768,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -758,7 +779,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="63" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -769,7 +790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" s="11" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
         <v>13</v>
       </c>
@@ -780,7 +801,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" s="11" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>36</v>
       </c>
@@ -789,7 +810,7 @@
       </c>
       <c r="C10" s="7"/>
     </row>
-    <row r="11" spans="1:6" s="11" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" s="11" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
         <v>34</v>
       </c>
@@ -798,7 +819,7 @@
       </c>
       <c r="C11" s="7"/>
     </row>
-    <row r="12" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>30</v>
       </c>
@@ -807,7 +828,7 @@
       </c>
       <c r="C12" s="1"/>
     </row>
-    <row r="16" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -827,7 +848,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="63" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -859,480 +880,434 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1690F214-8FDE-4731-8FEA-1D59D092703F}">
   <dimension ref="A3:Q20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K10" sqref="K10:M10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="18.33203125" customWidth="1"/>
     <col min="7" max="8" width="11" customWidth="1"/>
+    <col min="14" max="14" width="18.83203125" customWidth="1"/>
+    <col min="15" max="15" width="38.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B3" s="14" t="s">
+    <row r="3" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="8"/>
+      <c r="B3" s="18" t="s">
         <v>14</v>
       </c>
       <c r="C3" s="13"/>
       <c r="D3" s="13"/>
       <c r="E3" s="13"/>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14" t="s">
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14" t="s">
+      <c r="J3" s="18"/>
+      <c r="K3" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14" t="s">
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="O3" s="14"/>
-      <c r="P3" s="14" t="s">
+      <c r="O3" s="20"/>
+      <c r="P3" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="Q3" s="14"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="Q3" s="18"/>
+    </row>
+    <row r="4" spans="1:17" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="18" t="s">
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18" t="s">
+      <c r="J4" s="13"/>
+      <c r="K4" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="O4" s="16"/>
+      <c r="P4" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q4" s="13"/>
+    </row>
+    <row r="5" spans="1:17" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" s="15"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="L4" s="18"/>
-      <c r="M4" s="18"/>
-      <c r="N4" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="O4" s="18"/>
-      <c r="P4" s="18" t="s">
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="O5" s="16"/>
+      <c r="P5" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q5" s="13"/>
+    </row>
+    <row r="6" spans="1:17" ht="41" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="O6" s="16"/>
+      <c r="P6" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q6" s="13"/>
+    </row>
+    <row r="7" spans="1:17" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="Q4" s="18"/>
-    </row>
-    <row r="5" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="G5" s="16"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="L5" s="18"/>
-      <c r="M5" s="18"/>
-      <c r="N5" s="18" t="s">
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="O7" s="16"/>
+      <c r="P7" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q7" s="13"/>
+    </row>
+    <row r="8" spans="1:17" ht="44" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="O8" s="16"/>
+      <c r="P8" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="O5" s="18"/>
-      <c r="P5" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q5" s="18"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="L6" s="18"/>
-      <c r="M6" s="18"/>
-      <c r="N6" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="O6" s="18"/>
-      <c r="P6" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q6" s="18"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="18"/>
-      <c r="N7" s="18"/>
-      <c r="O7" s="18"/>
-      <c r="P7" s="18"/>
-      <c r="Q7" s="18"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="18"/>
-      <c r="O8" s="18"/>
-      <c r="P8" s="18"/>
-      <c r="Q8" s="18"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="18"/>
-      <c r="M9" s="18"/>
-      <c r="N9" s="18"/>
-      <c r="O9" s="18"/>
-      <c r="P9" s="18"/>
-      <c r="Q9" s="18"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B10" s="19"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="18"/>
-      <c r="M10" s="18"/>
-      <c r="N10" s="18"/>
-      <c r="O10" s="18"/>
-      <c r="P10" s="18"/>
-      <c r="Q10" s="18"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="18"/>
-      <c r="L11" s="18"/>
-      <c r="M11" s="18"/>
-      <c r="N11" s="18"/>
-      <c r="O11" s="18"/>
-      <c r="P11" s="18"/>
-      <c r="Q11" s="18"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="18"/>
-      <c r="L12" s="18"/>
-      <c r="M12" s="18"/>
-      <c r="N12" s="18"/>
-      <c r="O12" s="18"/>
-      <c r="P12" s="18"/>
-      <c r="Q12" s="18"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="18"/>
-      <c r="L13" s="18"/>
-      <c r="M13" s="18"/>
-      <c r="N13" s="18"/>
-      <c r="O13" s="18"/>
-      <c r="P13" s="18"/>
-      <c r="Q13" s="18"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
-      <c r="J14" s="18"/>
-      <c r="K14" s="18"/>
-      <c r="L14" s="18"/>
-      <c r="M14" s="18"/>
-      <c r="N14" s="18"/>
-      <c r="O14" s="18"/>
-      <c r="P14" s="18"/>
-      <c r="Q14" s="18"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="18"/>
-      <c r="J15" s="18"/>
-      <c r="K15" s="18"/>
-      <c r="L15" s="18"/>
-      <c r="M15" s="18"/>
-      <c r="N15" s="18"/>
-      <c r="O15" s="18"/>
-      <c r="P15" s="18"/>
-      <c r="Q15" s="18"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="18"/>
-      <c r="J16" s="18"/>
-      <c r="K16" s="18"/>
-      <c r="L16" s="18"/>
-      <c r="M16" s="18"/>
-      <c r="N16" s="18"/>
-      <c r="O16" s="18"/>
-      <c r="P16" s="18"/>
-      <c r="Q16" s="18"/>
-    </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="18"/>
-      <c r="J17" s="18"/>
-      <c r="K17" s="18"/>
-      <c r="L17" s="18"/>
-      <c r="M17" s="18"/>
-      <c r="N17" s="18"/>
-      <c r="O17" s="18"/>
-      <c r="P17" s="18"/>
-      <c r="Q17" s="18"/>
-    </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="18"/>
-      <c r="I18" s="18"/>
-      <c r="J18" s="18"/>
-      <c r="K18" s="18"/>
-      <c r="L18" s="18"/>
-      <c r="M18" s="18"/>
-      <c r="N18" s="18"/>
-      <c r="O18" s="18"/>
-      <c r="P18" s="18"/>
-      <c r="Q18" s="18"/>
-    </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="18"/>
-      <c r="L19" s="18"/>
-      <c r="M19" s="18"/>
-      <c r="N19" s="18"/>
-      <c r="O19" s="18"/>
-      <c r="P19" s="18"/>
-      <c r="Q19" s="18"/>
-    </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
-      <c r="K20" s="18"/>
-      <c r="L20" s="18"/>
-      <c r="M20" s="18"/>
-      <c r="N20" s="18"/>
-      <c r="O20" s="18"/>
-      <c r="P20" s="18"/>
-      <c r="Q20" s="18"/>
+      <c r="Q8" s="13"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="14"/>
+      <c r="O9" s="16"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="13"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="14"/>
+      <c r="O10" s="16"/>
+      <c r="P10" s="13"/>
+      <c r="Q10" s="13"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="14"/>
+      <c r="O11" s="16"/>
+      <c r="P11" s="13"/>
+      <c r="Q11" s="13"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="14"/>
+      <c r="O12" s="16"/>
+      <c r="P12" s="13"/>
+      <c r="Q12" s="13"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="14"/>
+      <c r="O13" s="16"/>
+      <c r="P13" s="13"/>
+      <c r="Q13" s="13"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="14"/>
+      <c r="O14" s="16"/>
+      <c r="P14" s="13"/>
+      <c r="Q14" s="13"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="14"/>
+      <c r="O15" s="16"/>
+      <c r="P15" s="13"/>
+      <c r="Q15" s="13"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="13"/>
+      <c r="N16" s="14"/>
+      <c r="O16" s="16"/>
+      <c r="P16" s="13"/>
+      <c r="Q16" s="13"/>
+    </row>
+    <row r="17" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="13"/>
+      <c r="N17" s="14"/>
+      <c r="O17" s="16"/>
+      <c r="P17" s="13"/>
+      <c r="Q17" s="13"/>
+    </row>
+    <row r="18" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="13"/>
+      <c r="M18" s="13"/>
+      <c r="N18" s="14"/>
+      <c r="O18" s="16"/>
+      <c r="P18" s="13"/>
+      <c r="Q18" s="13"/>
+    </row>
+    <row r="19" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="13"/>
+      <c r="N19" s="14"/>
+      <c r="O19" s="16"/>
+      <c r="P19" s="13"/>
+      <c r="Q19" s="13"/>
+    </row>
+    <row r="20" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="13"/>
+      <c r="N20" s="14"/>
+      <c r="O20" s="16"/>
+      <c r="P20" s="13"/>
+      <c r="Q20" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="108">
-    <mergeCell ref="P15:Q15"/>
-    <mergeCell ref="P16:Q16"/>
-    <mergeCell ref="P17:Q17"/>
-    <mergeCell ref="P18:Q18"/>
-    <mergeCell ref="P19:Q19"/>
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="P9:Q9"/>
-    <mergeCell ref="P10:Q10"/>
-    <mergeCell ref="P11:Q11"/>
-    <mergeCell ref="P12:Q12"/>
-    <mergeCell ref="P13:Q13"/>
-    <mergeCell ref="P14:Q14"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="P8:Q8"/>
-    <mergeCell ref="N15:O15"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="N19:O19"/>
-    <mergeCell ref="N20:O20"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="N12:O12"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="N14:O14"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="N8:O8"/>
-    <mergeCell ref="K15:M15"/>
-    <mergeCell ref="K16:M16"/>
-    <mergeCell ref="K17:M17"/>
-    <mergeCell ref="K18:M18"/>
-    <mergeCell ref="K19:M19"/>
-    <mergeCell ref="K20:M20"/>
-    <mergeCell ref="K9:M9"/>
-    <mergeCell ref="K10:M10"/>
-    <mergeCell ref="K11:M11"/>
-    <mergeCell ref="K12:M12"/>
-    <mergeCell ref="K13:M13"/>
-    <mergeCell ref="K14:M14"/>
-    <mergeCell ref="K3:M3"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="K5:M5"/>
-    <mergeCell ref="K6:M6"/>
-    <mergeCell ref="K7:M7"/>
-    <mergeCell ref="K8:M8"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
     <mergeCell ref="B19:E19"/>
     <mergeCell ref="B20:E20"/>
     <mergeCell ref="F3:H3"/>
@@ -1357,8 +1332,88 @@
     <mergeCell ref="B11:E11"/>
     <mergeCell ref="B12:E12"/>
     <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="K7:M7"/>
+    <mergeCell ref="K8:M8"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="K15:M15"/>
+    <mergeCell ref="K16:M16"/>
+    <mergeCell ref="K17:M17"/>
+    <mergeCell ref="K18:M18"/>
+    <mergeCell ref="K19:M19"/>
+    <mergeCell ref="K20:M20"/>
+    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="K10:M10"/>
+    <mergeCell ref="K11:M11"/>
+    <mergeCell ref="K12:M12"/>
+    <mergeCell ref="K13:M13"/>
+    <mergeCell ref="K14:M14"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="N19:O19"/>
+    <mergeCell ref="N20:O20"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="N12:O12"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="N14:O14"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="P8:Q8"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="P15:Q15"/>
+    <mergeCell ref="P16:Q16"/>
+    <mergeCell ref="P17:Q17"/>
+    <mergeCell ref="P18:Q18"/>
+    <mergeCell ref="P19:Q19"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="P9:Q9"/>
+    <mergeCell ref="P10:Q10"/>
+    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="P12:Q12"/>
+    <mergeCell ref="P13:Q13"/>
+    <mergeCell ref="P14:Q14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -1373,12 +1428,12 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="43.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
@@ -1389,14 +1444,14 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
     </row>
-    <row r="3" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Se modifica estimulo del requerimiento de usabilidad del navegador
</commit_message>
<xml_diff>
--- a/taller arq.xlsx
+++ b/taller arq.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nelsonpinzon/Library/Mobile Documents/com~apple~CloudDocs/Documents/Especialización/Arquitectura de Software/Software-Architecture/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76E34344-8234-CD40-B3C6-82652A126FBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A998C662-69A5-D647-AF57-D1B9D5E508C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{930C2BC0-64CF-D141-82C4-9B5BCF2C150D}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="27660" windowHeight="17500" activeTab="1" xr2:uid="{930C2BC0-64CF-D141-82C4-9B5BCF2C150D}"/>
   </bookViews>
   <sheets>
     <sheet name="QA" sheetId="1" r:id="rId1"/>
@@ -165,9 +165,6 @@
     <t>Componente defectuoso</t>
   </si>
   <si>
-    <t>No se muestra la aplicación para la ultima versión de chrome</t>
-  </si>
-  <si>
     <t>Verificar si la plicación funciona bajo esta version de navegador</t>
   </si>
   <si>
@@ -220,6 +217,9 @@
   </si>
   <si>
     <t>Notificar al area de servidor</t>
+  </si>
+  <si>
+    <t>fallo en el navegador</t>
   </si>
 </sst>
 </file>
@@ -355,6 +355,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -366,9 +369,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -692,7 +692,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30A29C82-537D-0A41-8469-EA9B4533FFF4}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -881,7 +881,7 @@
   <dimension ref="A3:Q20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N26" sqref="N26"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -894,65 +894,65 @@
   <sheetData>
     <row r="3" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8"/>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="14" t="s">
         <v>14</v>
       </c>
       <c r="C3" s="13"/>
       <c r="D3" s="13"/>
       <c r="E3" s="13"/>
-      <c r="F3" s="18" t="s">
+      <c r="F3" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18" t="s">
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18" t="s">
+      <c r="J3" s="14"/>
+      <c r="K3" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="L3" s="18"/>
-      <c r="M3" s="18"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
       <c r="N3" s="19" t="s">
         <v>18</v>
       </c>
       <c r="O3" s="20"/>
-      <c r="P3" s="18" t="s">
+      <c r="P3" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="Q3" s="18"/>
+      <c r="Q3" s="14"/>
     </row>
     <row r="4" spans="1:17" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="17"/>
       <c r="F4" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G4" s="13"/>
       <c r="H4" s="13"/>
       <c r="I4" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J4" s="13"/>
       <c r="K4" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L4" s="13"/>
       <c r="M4" s="13"/>
-      <c r="N4" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="O4" s="16"/>
+      <c r="N4" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="O4" s="17"/>
       <c r="P4" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="Q4" s="13"/>
     </row>
@@ -966,26 +966,26 @@
       <c r="C5" s="13"/>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
-      <c r="F5" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="G5" s="15"/>
-      <c r="H5" s="16"/>
+      <c r="F5" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="G5" s="16"/>
+      <c r="H5" s="17"/>
       <c r="I5" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J5" s="13"/>
       <c r="K5" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L5" s="13"/>
       <c r="M5" s="13"/>
-      <c r="N5" s="14" t="s">
+      <c r="N5" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="O5" s="17"/>
+      <c r="P5" s="13" t="s">
         <v>44</v>
-      </c>
-      <c r="O5" s="16"/>
-      <c r="P5" s="13" t="s">
-        <v>45</v>
       </c>
       <c r="Q5" s="13"/>
     </row>
@@ -1000,25 +1000,25 @@
       <c r="D6" s="13"/>
       <c r="E6" s="13"/>
       <c r="F6" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G6" s="13"/>
       <c r="H6" s="13"/>
       <c r="I6" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J6" s="13"/>
       <c r="K6" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L6" s="13"/>
       <c r="M6" s="13"/>
-      <c r="N6" s="14" t="s">
+      <c r="N6" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="O6" s="17"/>
+      <c r="P6" s="13" t="s">
         <v>48</v>
-      </c>
-      <c r="O6" s="16"/>
-      <c r="P6" s="13" t="s">
-        <v>49</v>
       </c>
       <c r="Q6" s="13"/>
     </row>
@@ -1033,31 +1033,31 @@
       <c r="D7" s="13"/>
       <c r="E7" s="13"/>
       <c r="F7" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
       <c r="I7" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J7" s="13"/>
       <c r="K7" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L7" s="13"/>
       <c r="M7" s="13"/>
-      <c r="N7" s="14" t="s">
+      <c r="N7" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="O7" s="17"/>
+      <c r="P7" s="13" t="s">
         <v>56</v>
-      </c>
-      <c r="O7" s="16"/>
-      <c r="P7" s="13" t="s">
-        <v>57</v>
       </c>
       <c r="Q7" s="13"/>
     </row>
     <row r="8" spans="1:17" ht="44" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B8" s="13" t="s">
         <v>41</v>
@@ -1066,25 +1066,25 @@
       <c r="D8" s="13"/>
       <c r="E8" s="13"/>
       <c r="F8" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G8" s="13"/>
       <c r="H8" s="13"/>
       <c r="I8" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J8" s="13"/>
       <c r="K8" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L8" s="13"/>
       <c r="M8" s="13"/>
-      <c r="N8" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="O8" s="16"/>
+      <c r="N8" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="O8" s="17"/>
       <c r="P8" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q8" s="13"/>
     </row>
@@ -1101,16 +1101,16 @@
       <c r="K9" s="13"/>
       <c r="L9" s="13"/>
       <c r="M9" s="13"/>
-      <c r="N9" s="14"/>
-      <c r="O9" s="16"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="17"/>
       <c r="P9" s="13"/>
       <c r="Q9" s="13"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
       <c r="F10" s="13"/>
       <c r="G10" s="13"/>
       <c r="H10" s="13"/>
@@ -1119,8 +1119,8 @@
       <c r="K10" s="13"/>
       <c r="L10" s="13"/>
       <c r="M10" s="13"/>
-      <c r="N10" s="14"/>
-      <c r="O10" s="16"/>
+      <c r="N10" s="15"/>
+      <c r="O10" s="17"/>
       <c r="P10" s="13"/>
       <c r="Q10" s="13"/>
     </row>
@@ -1137,8 +1137,8 @@
       <c r="K11" s="13"/>
       <c r="L11" s="13"/>
       <c r="M11" s="13"/>
-      <c r="N11" s="14"/>
-      <c r="O11" s="16"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="17"/>
       <c r="P11" s="13"/>
       <c r="Q11" s="13"/>
     </row>
@@ -1155,8 +1155,8 @@
       <c r="K12" s="13"/>
       <c r="L12" s="13"/>
       <c r="M12" s="13"/>
-      <c r="N12" s="14"/>
-      <c r="O12" s="16"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="17"/>
       <c r="P12" s="13"/>
       <c r="Q12" s="13"/>
     </row>
@@ -1173,8 +1173,8 @@
       <c r="K13" s="13"/>
       <c r="L13" s="13"/>
       <c r="M13" s="13"/>
-      <c r="N13" s="14"/>
-      <c r="O13" s="16"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="17"/>
       <c r="P13" s="13"/>
       <c r="Q13" s="13"/>
     </row>
@@ -1191,8 +1191,8 @@
       <c r="K14" s="13"/>
       <c r="L14" s="13"/>
       <c r="M14" s="13"/>
-      <c r="N14" s="14"/>
-      <c r="O14" s="16"/>
+      <c r="N14" s="15"/>
+      <c r="O14" s="17"/>
       <c r="P14" s="13"/>
       <c r="Q14" s="13"/>
     </row>
@@ -1209,8 +1209,8 @@
       <c r="K15" s="13"/>
       <c r="L15" s="13"/>
       <c r="M15" s="13"/>
-      <c r="N15" s="14"/>
-      <c r="O15" s="16"/>
+      <c r="N15" s="15"/>
+      <c r="O15" s="17"/>
       <c r="P15" s="13"/>
       <c r="Q15" s="13"/>
     </row>
@@ -1227,8 +1227,8 @@
       <c r="K16" s="13"/>
       <c r="L16" s="13"/>
       <c r="M16" s="13"/>
-      <c r="N16" s="14"/>
-      <c r="O16" s="16"/>
+      <c r="N16" s="15"/>
+      <c r="O16" s="17"/>
       <c r="P16" s="13"/>
       <c r="Q16" s="13"/>
     </row>
@@ -1245,8 +1245,8 @@
       <c r="K17" s="13"/>
       <c r="L17" s="13"/>
       <c r="M17" s="13"/>
-      <c r="N17" s="14"/>
-      <c r="O17" s="16"/>
+      <c r="N17" s="15"/>
+      <c r="O17" s="17"/>
       <c r="P17" s="13"/>
       <c r="Q17" s="13"/>
     </row>
@@ -1263,8 +1263,8 @@
       <c r="K18" s="13"/>
       <c r="L18" s="13"/>
       <c r="M18" s="13"/>
-      <c r="N18" s="14"/>
-      <c r="O18" s="16"/>
+      <c r="N18" s="15"/>
+      <c r="O18" s="17"/>
       <c r="P18" s="13"/>
       <c r="Q18" s="13"/>
     </row>
@@ -1281,8 +1281,8 @@
       <c r="K19" s="13"/>
       <c r="L19" s="13"/>
       <c r="M19" s="13"/>
-      <c r="N19" s="14"/>
-      <c r="O19" s="16"/>
+      <c r="N19" s="15"/>
+      <c r="O19" s="17"/>
       <c r="P19" s="13"/>
       <c r="Q19" s="13"/>
     </row>
@@ -1299,13 +1299,97 @@
       <c r="K20" s="13"/>
       <c r="L20" s="13"/>
       <c r="M20" s="13"/>
-      <c r="N20" s="14"/>
-      <c r="O20" s="16"/>
+      <c r="N20" s="15"/>
+      <c r="O20" s="17"/>
       <c r="P20" s="13"/>
       <c r="Q20" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="108">
+    <mergeCell ref="P18:Q18"/>
+    <mergeCell ref="P19:Q19"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="P9:Q9"/>
+    <mergeCell ref="P10:Q10"/>
+    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="P12:Q12"/>
+    <mergeCell ref="P13:Q13"/>
+    <mergeCell ref="P14:Q14"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="P8:Q8"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="P15:Q15"/>
+    <mergeCell ref="P16:Q16"/>
+    <mergeCell ref="P17:Q17"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="N19:O19"/>
+    <mergeCell ref="N20:O20"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="N12:O12"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="N14:O14"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="K15:M15"/>
+    <mergeCell ref="K16:M16"/>
+    <mergeCell ref="K17:M17"/>
+    <mergeCell ref="K18:M18"/>
+    <mergeCell ref="K19:M19"/>
+    <mergeCell ref="K20:M20"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="K7:M7"/>
+    <mergeCell ref="K8:M8"/>
+    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="K10:M10"/>
+    <mergeCell ref="K11:M11"/>
+    <mergeCell ref="K12:M12"/>
+    <mergeCell ref="K13:M13"/>
+    <mergeCell ref="K14:M14"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="I11:J11"/>
     <mergeCell ref="B7:E7"/>
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="B19:E19"/>
@@ -1330,90 +1414,6 @@
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="K3:M3"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="K5:M5"/>
-    <mergeCell ref="K6:M6"/>
-    <mergeCell ref="K7:M7"/>
-    <mergeCell ref="K8:M8"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="K15:M15"/>
-    <mergeCell ref="K16:M16"/>
-    <mergeCell ref="K17:M17"/>
-    <mergeCell ref="K18:M18"/>
-    <mergeCell ref="K19:M19"/>
-    <mergeCell ref="K20:M20"/>
-    <mergeCell ref="K9:M9"/>
-    <mergeCell ref="K10:M10"/>
-    <mergeCell ref="K11:M11"/>
-    <mergeCell ref="K12:M12"/>
-    <mergeCell ref="K13:M13"/>
-    <mergeCell ref="K14:M14"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="N19:O19"/>
-    <mergeCell ref="N20:O20"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="N12:O12"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="N14:O14"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="P8:Q8"/>
-    <mergeCell ref="N15:O15"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="N8:O8"/>
-    <mergeCell ref="P15:Q15"/>
-    <mergeCell ref="P16:Q16"/>
-    <mergeCell ref="P17:Q17"/>
-    <mergeCell ref="P18:Q18"/>
-    <mergeCell ref="P19:Q19"/>
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="P9:Q9"/>
-    <mergeCell ref="P10:Q10"/>
-    <mergeCell ref="P11:Q11"/>
-    <mergeCell ref="P12:Q12"/>
-    <mergeCell ref="P13:Q13"/>
-    <mergeCell ref="P14:Q14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>